<commit_message>
moved quint kalieds to M1/M2   and moved mines from M1/M2 to B2.  timed heavens;  added 10 sec buffer to heavens prem proj
</commit_message>
<xml_diff>
--- a/choreo/SateliteDiagram.xlsx
+++ b/choreo/SateliteDiagram.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="237">
   <si>
     <t>B1</t>
   </si>
@@ -75,10 +75,19 @@
     <t>mines</t>
   </si>
   <si>
+    <t>emperors tattoo</t>
+  </si>
+  <si>
+    <t>over the rainbow</t>
+  </si>
+  <si>
     <t>NOTES</t>
   </si>
   <si>
     <t>M1 / M2 shot 1)      one up and one angles toward B1/2</t>
+  </si>
+  <si>
+    <t>sunrise fountain</t>
   </si>
   <si>
     <t>M2 shot 3)   wired to front and center</t>
@@ -529,9 +538,6 @@
     <t>15) golden eye (pair #4a)</t>
   </si>
   <si>
-    <t>16) mines</t>
-  </si>
-  <si>
     <t>17) blistering cactus</t>
   </si>
   <si>
@@ -635,12 +641,6 @@
     <t>9) over the rainbow</t>
   </si>
   <si>
-    <t>10) 91 shot kaliedoscope (quint)</t>
-  </si>
-  <si>
-    <t>11) 91 shot kaliedoscope (quint)</t>
-  </si>
-  <si>
     <t>12) sunrise fountain</t>
   </si>
   <si>
@@ -656,12 +656,6 @@
     <t>17) silver monster</t>
   </si>
   <si>
-    <t>18) silver monster</t>
-  </si>
-  <si>
-    <t>19) meltdown</t>
-  </si>
-  <si>
     <t>20) Medusa</t>
   </si>
   <si>
@@ -750,6 +744,133 @@
   </si>
   <si>
     <t>CONES</t>
+  </si>
+  <si>
+    <t>Heavens</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2) 91 shot kalied</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(#1&amp;#2)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3) 91 shot kalied</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(#1&amp;#2)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2) 91 shot kalied</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(#3&amp;#4&amp;#5)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3) 91 shot kalied</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (#3&amp;#4&amp;#5)</t>
+    </r>
+  </si>
+  <si>
+    <t>18) meltdown</t>
+  </si>
+  <si>
+    <t>19) silver monster</t>
   </si>
 </sst>
 </file>
@@ -910,7 +1031,7 @@
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -920,7 +1041,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1241,7 +1361,7 @@
   <dimension ref="A1:AH51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="AC39" sqref="AC39"/>
+      <selection activeCell="AB15" sqref="AB15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1260,7 +1380,7 @@
     <col min="12" max="12" width="29.85546875" customWidth="1"/>
     <col min="13" max="13" width="26.7109375" customWidth="1"/>
     <col min="14" max="14" width="2" customWidth="1"/>
-    <col min="15" max="15" width="23.28515625" customWidth="1"/>
+    <col min="15" max="15" width="28" customWidth="1"/>
     <col min="16" max="16" width="1.85546875" customWidth="1"/>
     <col min="17" max="17" width="33.42578125" customWidth="1"/>
     <col min="18" max="18" width="25.140625" customWidth="1"/>
@@ -1270,27 +1390,38 @@
     <col min="22" max="22" width="28.140625" customWidth="1"/>
     <col min="23" max="23" width="1.28515625" customWidth="1"/>
     <col min="24" max="24" width="19.140625" customWidth="1"/>
+    <col min="26" max="26" width="11" customWidth="1"/>
+    <col min="27" max="27" width="17.7109375" customWidth="1"/>
     <col min="32" max="32" width="24.28515625" customWidth="1"/>
     <col min="33" max="33" width="79.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="Z1" s="18" t="s">
-        <v>231</v>
-      </c>
-      <c r="AA1" s="18"/>
-      <c r="AB1" s="18"/>
-      <c r="AC1" s="18"/>
-      <c r="AE1" s="17" t="s">
+      <c r="Z1" s="17" t="s">
+        <v>229</v>
+      </c>
+      <c r="AA1" s="17"/>
+      <c r="AB1" s="17"/>
+      <c r="AC1" s="17"/>
+      <c r="AE1" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="AF1" s="16"/>
+      <c r="AG1" s="16"/>
+      <c r="AH1" s="16"/>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="Z2" t="s">
+        <v>230</v>
+      </c>
+      <c r="AA2" t="s">
         <v>19</v>
       </c>
-      <c r="AF1" s="17"/>
-      <c r="AG1" s="17"/>
-      <c r="AH1" s="17"/>
-    </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AB2" t="s">
+        <v>7</v>
+      </c>
       <c r="AG2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.25">
@@ -1324,667 +1455,745 @@
       <c r="X3" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="AA3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>5</v>
+      </c>
       <c r="AG3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="C4" s="4"/>
       <c r="G4" s="4" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="L4" s="16" t="s">
-        <v>184</v>
+        <v>92</v>
+      </c>
+      <c r="L4" s="15" t="s">
+        <v>186</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="V4" s="4"/>
       <c r="X4" s="4"/>
+      <c r="AA4" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>0</v>
+      </c>
       <c r="AG4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="AH4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="C5" s="5"/>
       <c r="G5" s="4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="L5" s="16" t="s">
-        <v>185</v>
+        <v>93</v>
+      </c>
+      <c r="L5" s="15" t="s">
+        <v>187</v>
       </c>
       <c r="Q5" s="4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="V5" s="5"/>
       <c r="X5" s="5"/>
+      <c r="AA5" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>6</v>
+      </c>
       <c r="AG5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="AH5" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="C6" s="4" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="L6" s="16" t="s">
-        <v>186</v>
+        <v>94</v>
+      </c>
+      <c r="L6" s="15" t="s">
+        <v>188</v>
       </c>
       <c r="Q6" s="4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="R6" s="6" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="V6" s="4" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="X6" s="4"/>
+      <c r="AA6" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>4</v>
+      </c>
       <c r="AG6" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="AH6" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
-      <c r="C7" s="13" t="s">
-        <v>113</v>
+      <c r="C7" s="12" t="s">
+        <v>116</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Q7" s="5" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="R7" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="V7" s="13" t="s">
-        <v>113</v>
+        <v>95</v>
+      </c>
+      <c r="V7" s="12" t="s">
+        <v>116</v>
       </c>
       <c r="X7" s="5"/>
+      <c r="AA7" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>0</v>
+      </c>
       <c r="AG7" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="AH7" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="C8" s="4" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>8</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>3</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="O8" s="2" t="s">
         <v>2</v>
       </c>
       <c r="Q8" s="5" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="R8" s="6" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="T8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="V8" s="4" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="X8" s="4"/>
+      <c r="AA8" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>6</v>
+      </c>
       <c r="AG8" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="AH8" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="J9" s="3"/>
       <c r="L9" s="4" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="O9" s="3"/>
       <c r="Q9" s="5" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="R9" s="6" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="T9" s="3" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="V9" s="4" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="X9" s="5" t="s">
-        <v>110</v>
+        <v>113</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>4</v>
       </c>
       <c r="AG9" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="AH9" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>125</v>
+        <v>119</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>128</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="O10" s="8" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="Q10" s="5" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="R10" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="T10" s="12" t="s">
-        <v>148</v>
+        <v>74</v>
+      </c>
+      <c r="T10" s="11" t="s">
+        <v>151</v>
       </c>
       <c r="V10" s="4" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="X10" s="5" t="s">
-        <v>111</v>
+        <v>114</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>0</v>
       </c>
       <c r="AG10" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="AH10" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="C11" s="5" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>150</v>
+        <v>75</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>231</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="O11" s="7" t="s">
-        <v>172</v>
+        <v>193</v>
+      </c>
+      <c r="O11" s="6" t="s">
+        <v>233</v>
       </c>
       <c r="Q11" s="5" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="R11" s="6" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="T11" s="6" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="V11" s="5" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="X11" s="5"/>
+      <c r="AA11" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>8</v>
+      </c>
       <c r="AG11" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="C12" s="5" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="J12" s="7" t="s">
-        <v>151</v>
+        <v>97</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>232</v>
       </c>
       <c r="L12" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="O12" s="7" t="s">
-        <v>173</v>
+        <v>194</v>
+      </c>
+      <c r="O12" s="6" t="s">
+        <v>234</v>
       </c>
       <c r="Q12" s="4" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="R12" s="3" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="T12" s="6" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="V12" s="5" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="X12" s="5"/>
+      <c r="AA12" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>10</v>
+      </c>
       <c r="AG12" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="C13" s="5" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>95</v>
+        <v>77</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>98</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="L13" s="9" t="s">
-        <v>193</v>
+        <v>153</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>195</v>
       </c>
       <c r="O13" s="7" t="s">
         <v>174</v>
       </c>
       <c r="Q13" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="R13" s="11" t="s">
-        <v>109</v>
+        <v>77</v>
+      </c>
+      <c r="R13" s="10" t="s">
+        <v>112</v>
       </c>
       <c r="T13" s="3" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="V13" s="5" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="X13" s="5"/>
+      <c r="AA13" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>0</v>
+      </c>
       <c r="AG13" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="AH13" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="C14" s="5" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="L14" s="9" t="s">
-        <v>194</v>
+        <v>154</v>
+      </c>
+      <c r="L14" s="5" t="s">
+        <v>139</v>
       </c>
       <c r="O14" s="7" t="s">
-        <v>153</v>
+        <v>175</v>
       </c>
       <c r="Q14" s="4" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="R14" s="3" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="T14" s="3" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="V14" s="5" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="X14" s="5"/>
+      <c r="AA14" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>8</v>
+      </c>
       <c r="AG14" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="AH14" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
-      <c r="C15" s="13" t="s">
-        <v>121</v>
+      <c r="C15" s="12" t="s">
+        <v>124</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="L15" s="5" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="O15" s="7" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="Q15" s="4" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="R15" s="3" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="T15" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="V15" s="13" t="s">
-        <v>121</v>
+        <v>133</v>
+      </c>
+      <c r="V15" s="12" t="s">
+        <v>124</v>
       </c>
       <c r="X15" s="5"/>
+      <c r="AA15" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>10</v>
+      </c>
       <c r="AE15" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="AF15" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="AG15" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="C16" s="5" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>136</v>
+        <v>197</v>
       </c>
       <c r="O16" s="7" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="Q16" s="4" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="R16" s="3" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="T16" s="3" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="V16" s="5" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="X16" s="5"/>
       <c r="AF16" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="AG16" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
-      <c r="C17" s="13" t="s">
-        <v>123</v>
+      <c r="C17" s="12" t="s">
+        <v>126</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="H17" s="12" t="s">
-        <v>98</v>
+        <v>81</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>101</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="L17" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="O17" s="8" t="s">
-        <v>176</v>
+        <v>198</v>
+      </c>
+      <c r="O17" s="7" t="s">
+        <v>177</v>
       </c>
       <c r="Q17" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="R17" s="12" t="s">
-        <v>98</v>
+        <v>81</v>
+      </c>
+      <c r="R17" s="11" t="s">
+        <v>101</v>
       </c>
       <c r="T17" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="V17" s="13" t="s">
-        <v>123</v>
+        <v>135</v>
+      </c>
+      <c r="V17" s="12" t="s">
+        <v>126</v>
       </c>
       <c r="X17" s="5"/>
       <c r="AF17" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="AG17" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="C18" s="5"/>
       <c r="E18" s="6" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="J18" s="8" t="s">
-        <v>157</v>
+        <v>102</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>158</v>
       </c>
       <c r="L18" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="O18" s="3" t="s">
-        <v>177</v>
+        <v>199</v>
+      </c>
+      <c r="O18" s="7" t="s">
+        <v>158</v>
       </c>
       <c r="Q18" s="4" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="R18" s="6" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="T18" s="6" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="V18" s="5"/>
       <c r="X18" s="5"/>
       <c r="AF18" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="AG18" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="C19" s="5"/>
       <c r="E19" s="6" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>158</v>
+        <v>103</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>159</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="O19" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="O19" s="8" t="s">
         <v>178</v>
       </c>
       <c r="Q19" s="5" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="R19" s="6" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="T19" s="6" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="V19" s="5"/>
       <c r="X19" s="5"/>
       <c r="AF19" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="AG19" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="AH19" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="C20" s="5"/>
       <c r="E20" s="6" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="J20" s="7" t="s">
-        <v>159</v>
+        <v>104</v>
+      </c>
+      <c r="J20" s="8" t="s">
+        <v>160</v>
       </c>
       <c r="L20" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="O20" s="12" t="s">
+        <v>236</v>
+      </c>
+      <c r="O20" s="3" t="s">
         <v>179</v>
       </c>
       <c r="Q20" s="5" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="R20" s="6" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="T20" s="6" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="V20" s="5"/>
       <c r="X20" s="5"/>
@@ -1993,67 +2202,67 @@
       <c r="A21" s="5"/>
       <c r="C21" s="5"/>
       <c r="E21" s="3" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="J21" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="L21" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="L21" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="O21" s="15" t="s">
+      <c r="O21" s="7" t="s">
         <v>180</v>
       </c>
       <c r="Q21" s="4" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="R21" s="3" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="T21" s="3" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="V21" s="5"/>
       <c r="X21" s="5"/>
       <c r="AE21" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="C22" s="5"/>
       <c r="E22" s="3" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="H22" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="J22" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="L22" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="H22" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="J22" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="L22" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="O22" s="15" t="s">
+      <c r="O22" s="11" t="s">
         <v>181</v>
       </c>
       <c r="Q22" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="R22" s="14" t="s">
-        <v>103</v>
+        <v>86</v>
+      </c>
+      <c r="R22" s="13" t="s">
+        <v>106</v>
       </c>
       <c r="T22" s="3" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="V22" s="5"/>
       <c r="X22" s="5"/>
@@ -2061,32 +2270,32 @@
     <row r="23" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="C23" s="5"/>
-      <c r="E23" s="12" t="s">
-        <v>138</v>
+      <c r="E23" s="11" t="s">
+        <v>141</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="J23" s="15" t="s">
-        <v>162</v>
+        <v>107</v>
+      </c>
+      <c r="J23" s="14" t="s">
+        <v>163</v>
       </c>
       <c r="L23" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="O23" s="15" t="s">
+      <c r="O23" s="14" t="s">
         <v>182</v>
       </c>
       <c r="Q23" s="5" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="R23" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="T23" s="12" t="s">
-        <v>138</v>
+        <v>107</v>
+      </c>
+      <c r="T23" s="11" t="s">
+        <v>141</v>
       </c>
       <c r="V23" s="5"/>
       <c r="X23" s="5"/>
@@ -2094,41 +2303,41 @@
         <v>18</v>
       </c>
       <c r="AG23" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="AH23" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="C24" s="5"/>
       <c r="E24" s="3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="J24" s="15" t="s">
-        <v>163</v>
-      </c>
-      <c r="L24" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="J24" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="L24" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="O24" s="15" t="s">
+      <c r="O24" s="14" t="s">
         <v>183</v>
       </c>
       <c r="Q24" s="5" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="R24" s="6" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="T24" s="3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="V24" s="5"/>
       <c r="X24" s="5"/>
@@ -2136,41 +2345,41 @@
         <v>18</v>
       </c>
       <c r="AG24" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="AH24" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="C25" s="5"/>
       <c r="E25" s="3" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="J25" s="8" t="s">
-        <v>164</v>
+        <v>109</v>
+      </c>
+      <c r="J25" s="14" t="s">
+        <v>165</v>
       </c>
       <c r="L25" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="O25" s="8" t="s">
-        <v>164</v>
+      <c r="O25" s="14" t="s">
+        <v>184</v>
       </c>
       <c r="Q25" s="5" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="R25" s="6" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="T25" s="3" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="V25" s="5"/>
       <c r="X25" s="5"/>
@@ -2178,41 +2387,41 @@
         <v>13</v>
       </c>
       <c r="AG25" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="AH25" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="C26" s="5"/>
       <c r="E26" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="J26" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="L26" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="J26" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="L26" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="O26" s="8" t="s">
-        <v>165</v>
+      <c r="O26" s="14" t="s">
+        <v>185</v>
       </c>
       <c r="Q26" s="5" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="R26" s="6" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="T26" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="V26" s="5"/>
       <c r="X26" s="5"/>
@@ -2220,41 +2429,41 @@
         <v>13</v>
       </c>
       <c r="AG26" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="AH26" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="C27" s="5"/>
       <c r="E27" s="3" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="J27" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="L27" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="L27" s="5" t="s">
         <v>206</v>
       </c>
       <c r="O27" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="Q27" s="5" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="R27" s="6" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="T27" s="3" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="V27" s="5"/>
       <c r="X27" s="5"/>
@@ -2262,136 +2471,140 @@
         <v>14</v>
       </c>
       <c r="AG27" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="AH27" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:34" x14ac:dyDescent="0.25">
       <c r="E28" s="6" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="J28" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="M28" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="M28" s="5" t="s">
         <v>207</v>
       </c>
       <c r="O28" s="8" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="T28" s="6" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="AF28" t="s">
         <v>14</v>
       </c>
       <c r="AG28" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="AH28" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:34" x14ac:dyDescent="0.25">
       <c r="E29" s="6" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="J29" s="8" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="M29" s="5" t="s">
         <v>208</v>
       </c>
       <c r="O29" s="8" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="T29" s="6" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="AF29" t="s">
         <v>15</v>
       </c>
       <c r="AG29" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="AH29" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:34" x14ac:dyDescent="0.25">
       <c r="E30" s="6" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="J30" s="8" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="M30" s="5" t="s">
         <v>209</v>
       </c>
       <c r="O30" s="8" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="T30" s="6" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="AF30" t="s">
         <v>15</v>
       </c>
       <c r="AG30" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="AH30" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:34" x14ac:dyDescent="0.25">
       <c r="E31" s="6" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="J31" s="8" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="M31" s="5" t="s">
         <v>210</v>
       </c>
       <c r="O31" s="8" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="T31" s="6" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="AF31" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="AG31" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="AH31" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:34" x14ac:dyDescent="0.25">
       <c r="E32" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="J32" s="6"/>
+        <v>150</v>
+      </c>
+      <c r="J32" s="8" t="s">
+        <v>172</v>
+      </c>
       <c r="M32" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="O32" s="6"/>
+      <c r="O32" s="8" t="s">
+        <v>172</v>
+      </c>
       <c r="T32" s="6" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="AF32" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="AG32" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="AH32" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="33" spans="10:34" x14ac:dyDescent="0.25">
@@ -2401,41 +2614,41 @@
       </c>
       <c r="O33" s="6"/>
       <c r="AF33" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="AG33" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="AH33" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="34" spans="10:34" x14ac:dyDescent="0.25">
-      <c r="M34" s="5" t="s">
+      <c r="M34" s="4" t="s">
         <v>213</v>
       </c>
       <c r="AF34" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="AG34" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH34" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="10:34" x14ac:dyDescent="0.25">
+      <c r="M35" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="AF35" t="s">
         <v>59</v>
       </c>
-      <c r="AH34" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="35" spans="10:34" x14ac:dyDescent="0.25">
-      <c r="M35" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="AF35" t="s">
-        <v>56</v>
-      </c>
       <c r="AG35" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="AH35" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="36" spans="10:34" x14ac:dyDescent="0.25">
@@ -2443,13 +2656,13 @@
         <v>215</v>
       </c>
       <c r="AF36" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="AG36" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="AH36" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="37" spans="10:34" x14ac:dyDescent="0.25">
@@ -2457,10 +2670,10 @@
         <v>216</v>
       </c>
       <c r="AF37" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="AG37" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="38" spans="10:34" x14ac:dyDescent="0.25">
@@ -2468,10 +2681,10 @@
         <v>217</v>
       </c>
       <c r="AF38" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="AG38" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="39" spans="10:34" x14ac:dyDescent="0.25">
@@ -2482,22 +2695,23 @@
         <v>16</v>
       </c>
       <c r="AG39" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="40" spans="10:34" x14ac:dyDescent="0.25">
-      <c r="M40" s="4" t="s">
+      <c r="J40" s="6"/>
+      <c r="M40" s="5" t="s">
         <v>219</v>
       </c>
       <c r="AF40" t="s">
         <v>16</v>
       </c>
       <c r="AG40" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="41" spans="10:34" x14ac:dyDescent="0.25">
-      <c r="M41" s="4" t="s">
+      <c r="M41" s="5" t="s">
         <v>220</v>
       </c>
     </row>
@@ -2510,53 +2724,53 @@
       <c r="M43" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="AE43" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="AF43" s="19"/>
-      <c r="AG43" s="19"/>
+      <c r="AE43" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF43" s="18"/>
+      <c r="AG43" s="18"/>
     </row>
     <row r="44" spans="10:34" x14ac:dyDescent="0.25">
       <c r="M44" s="5" t="s">
         <v>223</v>
       </c>
       <c r="AE44" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="45" spans="10:34" x14ac:dyDescent="0.25">
       <c r="M45" s="5" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="46" spans="10:34" x14ac:dyDescent="0.25">
       <c r="M46" s="5" t="s">
-        <v>225</v>
+        <v>18</v>
       </c>
     </row>
     <row r="47" spans="10:34" x14ac:dyDescent="0.25">
       <c r="M47" s="5" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="48" spans="10:34" x14ac:dyDescent="0.25">
       <c r="M48" s="5" t="s">
-        <v>226</v>
+        <v>18</v>
       </c>
     </row>
     <row r="49" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M49" s="5" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="50" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M50" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="51" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M51" s="5" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
completed cuetimes for lost together; added cone data to sat diagrams, added 10 second buffer to lost together prem proj
</commit_message>
<xml_diff>
--- a/choreo/SateliteDiagram.xlsx
+++ b/choreo/SateliteDiagram.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="240">
   <si>
     <t>B1</t>
   </si>
@@ -871,6 +871,15 @@
   </si>
   <si>
     <t>19) silver monster</t>
+  </si>
+  <si>
+    <t>Lost</t>
+  </si>
+  <si>
+    <t>winter storm</t>
+  </si>
+  <si>
+    <t>14) ice storm (pair #2)</t>
   </si>
 </sst>
 </file>
@@ -1031,7 +1040,7 @@
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1051,6 +1060,7 @@
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1361,7 +1371,7 @@
   <dimension ref="A1:AH51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="AB15" sqref="AB15"/>
+      <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2034,6 +2044,15 @@
         <v>125</v>
       </c>
       <c r="X16" s="5"/>
+      <c r="Z16" t="s">
+        <v>237</v>
+      </c>
+      <c r="AA16" s="19" t="s">
+        <v>238</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>3</v>
+      </c>
       <c r="AF16" t="s">
         <v>38</v>
       </c>
@@ -2068,7 +2087,7 @@
         <v>81</v>
       </c>
       <c r="R17" s="11" t="s">
-        <v>101</v>
+        <v>239</v>
       </c>
       <c r="T17" s="6" t="s">
         <v>135</v>
@@ -2077,6 +2096,12 @@
         <v>126</v>
       </c>
       <c r="X17" s="5"/>
+      <c r="AA17" s="19" t="s">
+        <v>238</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>2</v>
+      </c>
       <c r="AF17" t="s">
         <v>46</v>
       </c>

</xml_diff>

<commit_message>
completed cuetimes for the oaf; updates sat diagrams, added 10 second buffer to The Oaf prem proj
</commit_message>
<xml_diff>
--- a/choreo/SateliteDiagram.xlsx
+++ b/choreo/SateliteDiagram.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="241">
   <si>
     <t>B1</t>
   </si>
@@ -880,6 +880,9 @@
   </si>
   <si>
     <t>14) ice storm (pair #2)</t>
+  </si>
+  <si>
+    <t>pirates bounty - separate shots #2 and #6 for other stations; direct wire to each row for individual control</t>
   </si>
 </sst>
 </file>
@@ -1056,11 +1059,11 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1371,7 +1374,7 @@
   <dimension ref="A1:AH51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="R17" sqref="R17"/>
+      <selection activeCell="AE44" sqref="AE44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1407,18 +1410,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="Z1" s="17" t="s">
+      <c r="Z1" s="16" t="s">
         <v>229</v>
       </c>
-      <c r="AA1" s="17"/>
-      <c r="AB1" s="17"/>
-      <c r="AC1" s="17"/>
-      <c r="AE1" s="16" t="s">
+      <c r="AA1" s="16"/>
+      <c r="AB1" s="16"/>
+      <c r="AC1" s="16"/>
+      <c r="AE1" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="AF1" s="16"/>
-      <c r="AG1" s="16"/>
-      <c r="AH1" s="16"/>
+      <c r="AF1" s="15"/>
+      <c r="AG1" s="15"/>
+      <c r="AH1" s="15"/>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="Z2" t="s">
@@ -1484,7 +1487,7 @@
       <c r="H4" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="L4" s="15" t="s">
+      <c r="L4" s="19" t="s">
         <v>186</v>
       </c>
       <c r="Q4" s="4" t="s">
@@ -1517,7 +1520,7 @@
       <c r="H5" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="L5" s="15" t="s">
+      <c r="L5" s="19" t="s">
         <v>187</v>
       </c>
       <c r="Q5" s="4" t="s">
@@ -1552,7 +1555,7 @@
       <c r="H6" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="L6" s="15" t="s">
+      <c r="L6" s="19" t="s">
         <v>188</v>
       </c>
       <c r="Q6" s="4" t="s">
@@ -1720,7 +1723,7 @@
       <c r="C10" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="13" t="s">
         <v>128</v>
       </c>
       <c r="G10" s="5" t="s">
@@ -1732,7 +1735,7 @@
       <c r="J10" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="L10" s="4" t="s">
+      <c r="L10" s="19" t="s">
         <v>192</v>
       </c>
       <c r="O10" s="8" t="s">
@@ -1744,7 +1747,7 @@
       <c r="R10" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="T10" s="11" t="s">
+      <c r="T10" s="13" t="s">
         <v>151</v>
       </c>
       <c r="V10" s="4" t="s">
@@ -2047,7 +2050,7 @@
       <c r="Z16" t="s">
         <v>237</v>
       </c>
-      <c r="AA16" s="19" t="s">
+      <c r="AA16" s="18" t="s">
         <v>238</v>
       </c>
       <c r="AB16" t="s">
@@ -2096,7 +2099,7 @@
         <v>126</v>
       </c>
       <c r="X17" s="5"/>
-      <c r="AA17" s="19" t="s">
+      <c r="AA17" s="18" t="s">
         <v>238</v>
       </c>
       <c r="AB17" t="s">
@@ -2749,23 +2752,26 @@
       <c r="M43" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="AE43" s="18" t="s">
+      <c r="AE43" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="AF43" s="18"/>
-      <c r="AG43" s="18"/>
+      <c r="AF43" s="17"/>
+      <c r="AG43" s="17"/>
     </row>
     <row r="44" spans="10:34" x14ac:dyDescent="0.25">
       <c r="M44" s="5" t="s">
         <v>223</v>
       </c>
       <c r="AE44" t="s">
-        <v>37</v>
+        <v>240</v>
       </c>
     </row>
     <row r="45" spans="10:34" x14ac:dyDescent="0.25">
       <c r="M45" s="5" t="s">
         <v>225</v>
+      </c>
+      <c r="AE45" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="46" spans="10:34" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
completed cuetimes for fiddlers; updates sat diagrams, added 10 second buffer to fiddlers prem proj
</commit_message>
<xml_diff>
--- a/choreo/SateliteDiagram.xlsx
+++ b/choreo/SateliteDiagram.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="242">
   <si>
     <t>B1</t>
   </si>
@@ -883,6 +883,9 @@
   </si>
   <si>
     <t>pirates bounty - separate shots #2 and #6 for other stations; direct wire to each row for individual control</t>
+  </si>
+  <si>
+    <t>Fiddlers</t>
   </si>
 </sst>
 </file>
@@ -1374,7 +1377,7 @@
   <dimension ref="A1:AH51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="AE44" sqref="AE44"/>
+      <selection activeCell="AH39" sqref="AH39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2144,6 +2147,15 @@
       </c>
       <c r="V18" s="5"/>
       <c r="X18" s="5"/>
+      <c r="Z18" t="s">
+        <v>241</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>8</v>
+      </c>
       <c r="AF18" t="s">
         <v>38</v>
       </c>
@@ -2183,6 +2195,12 @@
       </c>
       <c r="V19" s="5"/>
       <c r="X19" s="5"/>
+      <c r="AA19" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>10</v>
+      </c>
       <c r="AF19" t="s">
         <v>46</v>
       </c>
@@ -2225,6 +2243,12 @@
       </c>
       <c r="V20" s="5"/>
       <c r="X20" s="5"/>
+      <c r="AA20" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB20" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="21" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
@@ -2258,6 +2282,12 @@
       </c>
       <c r="V21" s="5"/>
       <c r="X21" s="5"/>
+      <c r="AA21" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>2</v>
+      </c>
       <c r="AE21" t="s">
         <v>47</v>
       </c>
@@ -2725,6 +2755,9 @@
       <c r="AG39" t="s">
         <v>63</v>
       </c>
+      <c r="AH39" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="40" spans="10:34" x14ac:dyDescent="0.25">
       <c r="J40" s="6"/>
@@ -2736,6 +2769,9 @@
       </c>
       <c r="AG40" t="s">
         <v>64</v>
+      </c>
+      <c r="AH40" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="41" spans="10:34" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
completed cuetimes for free world; updates sat diagrams, added 10 second buffer to free world prem proj
</commit_message>
<xml_diff>
--- a/choreo/SateliteDiagram.xlsx
+++ b/choreo/SateliteDiagram.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="240">
   <si>
     <t>B1</t>
   </si>
@@ -160,12 +160,6 @@
   </si>
   <si>
     <t>free world</t>
-  </si>
-  <si>
-    <t>M1 shot 16) wired to front and center</t>
-  </si>
-  <si>
-    <t>M2 shot 16) wired to front and center</t>
   </si>
   <si>
     <t>M1 shot 17) wired to water infront of M3/B3</t>
@@ -1377,7 +1371,7 @@
   <dimension ref="A1:AH51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="AH39" sqref="AH39"/>
+      <selection activeCell="AF23" sqref="AF23:AH24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1414,7 +1408,7 @@
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="Z1" s="16" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="AA1" s="16"/>
       <c r="AB1" s="16"/>
@@ -1428,7 +1422,7 @@
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="Z2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="AA2" t="s">
         <v>19</v>
@@ -1485,19 +1479,19 @@
       <c r="A4" s="4"/>
       <c r="C4" s="4"/>
       <c r="G4" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="L4" s="19" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="V4" s="4"/>
       <c r="X4" s="4"/>
@@ -1518,19 +1512,19 @@
       <c r="A5" s="5"/>
       <c r="C5" s="5"/>
       <c r="G5" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="L5" s="19" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="Q5" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="V5" s="5"/>
       <c r="X5" s="5"/>
@@ -1550,25 +1544,25 @@
     <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="C6" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="L6" s="19" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="Q6" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="R6" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="V6" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="X6" s="4"/>
       <c r="AA6" t="s">
@@ -1587,25 +1581,25 @@
     <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="C7" s="12" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="Q7" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="R7" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="V7" s="12" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="X7" s="5"/>
       <c r="AA7" t="s">
@@ -1624,37 +1618,37 @@
     <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="C8" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>8</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>3</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="O8" s="2" t="s">
         <v>2</v>
       </c>
       <c r="Q8" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="R8" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="T8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="V8" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="X8" s="4"/>
       <c r="AA8" t="s">
@@ -1672,39 +1666,39 @@
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J9" s="3"/>
       <c r="L9" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="O9" s="3"/>
       <c r="Q9" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="R9" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T9" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="V9" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="X9" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="AA9" t="s">
         <v>20</v>
@@ -1721,43 +1715,43 @@
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="L10" s="19" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="O10" s="8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="Q10" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="R10" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="T10" s="13" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="V10" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="X10" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="AA10" t="s">
         <v>23</v>
@@ -1775,37 +1769,37 @@
     <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="C11" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J11" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="O11" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="L11" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="O11" s="6" t="s">
-        <v>233</v>
-      </c>
       <c r="Q11" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="R11" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="T11" s="6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="V11" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="X11" s="5"/>
       <c r="AA11" t="s">
@@ -1821,37 +1815,37 @@
     <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="C12" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="J12" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="O12" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="L12" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="O12" s="6" t="s">
-        <v>234</v>
-      </c>
       <c r="Q12" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="R12" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="T12" s="6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="V12" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="X12" s="5"/>
       <c r="AA12" t="s">
@@ -1867,37 +1861,37 @@
     <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="C13" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="O13" s="7" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="Q13" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="R13" s="10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="T13" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="V13" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="X13" s="5"/>
       <c r="AA13" t="s">
@@ -1916,37 +1910,37 @@
     <row r="14" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="C14" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="O14" s="7" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="Q14" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="R14" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="T14" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="V14" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="X14" s="5"/>
       <c r="AA14" t="s">
@@ -1965,37 +1959,37 @@
     <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="C15" s="12" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="L15" s="5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="O15" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="Q15" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="R15" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="T15" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="V15" s="12" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="X15" s="5"/>
       <c r="AA15" t="s">
@@ -2017,44 +2011,44 @@
     <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="C16" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="O16" s="7" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="Q16" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="R16" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="T16" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="V16" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="X16" s="5"/>
       <c r="Z16" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="AA16" s="18" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="AB16" t="s">
         <v>3</v>
@@ -2069,41 +2063,41 @@
     <row r="17" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="C17" s="12" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L17" s="5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="O17" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Q17" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="R17" s="11" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="T17" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="V17" s="12" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="X17" s="5"/>
       <c r="AA17" s="18" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="AB17" t="s">
         <v>2</v>
@@ -2119,36 +2113,36 @@
       <c r="A18" s="5"/>
       <c r="C18" s="5"/>
       <c r="E18" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="L18" s="5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="O18" s="7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="Q18" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="R18" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="T18" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="V18" s="5"/>
       <c r="X18" s="5"/>
       <c r="Z18" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="AA18" t="s">
         <v>23</v>
@@ -2167,31 +2161,31 @@
       <c r="A19" s="5"/>
       <c r="C19" s="5"/>
       <c r="E19" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="O19" s="8" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="Q19" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="R19" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="T19" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="V19" s="5"/>
       <c r="X19" s="5"/>
@@ -2215,31 +2209,31 @@
       <c r="A20" s="5"/>
       <c r="C20" s="5"/>
       <c r="E20" s="6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="L20" s="5" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="O20" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="Q20" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="R20" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="T20" s="6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="V20" s="5"/>
       <c r="X20" s="5"/>
@@ -2254,31 +2248,31 @@
       <c r="A21" s="5"/>
       <c r="C21" s="5"/>
       <c r="E21" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="O21" s="7" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="Q21" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="R21" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="T21" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="V21" s="5"/>
       <c r="X21" s="5"/>
@@ -2296,148 +2290,151 @@
       <c r="A22" s="5"/>
       <c r="C22" s="5"/>
       <c r="E22" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H22" s="13" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="L22" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="O22" s="11" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="Q22" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="R22" s="13" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="T22" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="V22" s="5"/>
       <c r="X22" s="5"/>
+      <c r="Z22" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="C23" s="5"/>
       <c r="E23" s="11" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="J23" s="14" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="O23" s="14" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="Q23" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="R23" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="T23" s="11" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="V23" s="5"/>
       <c r="X23" s="5"/>
-      <c r="AF23" t="s">
-        <v>18</v>
-      </c>
-      <c r="AG23" t="s">
-        <v>48</v>
-      </c>
-      <c r="AH23" t="s">
-        <v>27</v>
+      <c r="AA23" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="C24" s="5"/>
       <c r="E24" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="J24" s="14" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="O24" s="14" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="Q24" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="R24" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="T24" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="V24" s="5"/>
       <c r="X24" s="5"/>
-      <c r="AF24" t="s">
-        <v>18</v>
-      </c>
-      <c r="AG24" t="s">
-        <v>49</v>
-      </c>
-      <c r="AH24" t="s">
-        <v>27</v>
+      <c r="AA24" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="C25" s="5"/>
       <c r="E25" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="J25" s="14" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="O25" s="14" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="Q25" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="R25" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="T25" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="V25" s="5"/>
       <c r="X25" s="5"/>
@@ -2445,7 +2442,7 @@
         <v>13</v>
       </c>
       <c r="AG25" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="AH25" t="s">
         <v>27</v>
@@ -2455,31 +2452,31 @@
       <c r="A26" s="5"/>
       <c r="C26" s="5"/>
       <c r="E26" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="J26" s="14" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="L26" s="9" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="O26" s="14" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="Q26" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="R26" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="T26" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="V26" s="5"/>
       <c r="X26" s="5"/>
@@ -2487,7 +2484,7 @@
         <v>13</v>
       </c>
       <c r="AG26" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="AH26" t="s">
         <v>27</v>
@@ -2497,31 +2494,31 @@
       <c r="A27" s="5"/>
       <c r="C27" s="5"/>
       <c r="E27" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="J27" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="L27" s="5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="O27" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="Q27" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="R27" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="T27" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="V27" s="5"/>
       <c r="X27" s="5"/>
@@ -2529,7 +2526,7 @@
         <v>14</v>
       </c>
       <c r="AG27" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AH27" t="s">
         <v>27</v>
@@ -2537,25 +2534,25 @@
     </row>
     <row r="28" spans="1:34" x14ac:dyDescent="0.25">
       <c r="E28" s="6" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="J28" s="8" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="M28" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="O28" s="8" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="T28" s="6" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AF28" t="s">
         <v>14</v>
       </c>
       <c r="AG28" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="AH28" t="s">
         <v>27</v>
@@ -2563,25 +2560,25 @@
     </row>
     <row r="29" spans="1:34" x14ac:dyDescent="0.25">
       <c r="E29" s="6" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="J29" s="8" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="M29" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="O29" s="8" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="T29" s="6" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AF29" t="s">
         <v>15</v>
       </c>
       <c r="AG29" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AH29" t="s">
         <v>27</v>
@@ -2589,25 +2586,25 @@
     </row>
     <row r="30" spans="1:34" x14ac:dyDescent="0.25">
       <c r="E30" s="6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="J30" s="8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="M30" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="O30" s="8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="T30" s="6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AF30" t="s">
         <v>15</v>
       </c>
       <c r="AG30" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AH30" t="s">
         <v>27</v>
@@ -2615,25 +2612,25 @@
     </row>
     <row r="31" spans="1:34" x14ac:dyDescent="0.25">
       <c r="E31" s="6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="J31" s="8" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="M31" s="5" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="O31" s="8" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="T31" s="6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="AF31" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AG31" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="AH31" t="s">
         <v>27</v>
@@ -2641,25 +2638,25 @@
     </row>
     <row r="32" spans="1:34" x14ac:dyDescent="0.25">
       <c r="E32" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J32" s="8" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="M32" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="O32" s="8" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="T32" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="AF32" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG32" t="s">
         <v>56</v>
-      </c>
-      <c r="AG32" t="s">
-        <v>58</v>
       </c>
       <c r="AH32" t="s">
         <v>27</v>
@@ -2668,14 +2665,14 @@
     <row r="33" spans="10:34" x14ac:dyDescent="0.25">
       <c r="J33" s="6"/>
       <c r="M33" s="5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="O33" s="6"/>
       <c r="AF33" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AG33" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="AH33" t="s">
         <v>27</v>
@@ -2683,13 +2680,13 @@
     </row>
     <row r="34" spans="10:34" x14ac:dyDescent="0.25">
       <c r="M34" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="AF34" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG34" t="s">
         <v>60</v>
-      </c>
-      <c r="AG34" t="s">
-        <v>62</v>
       </c>
       <c r="AH34" t="s">
         <v>27</v>
@@ -2697,13 +2694,13 @@
     </row>
     <row r="35" spans="10:34" x14ac:dyDescent="0.25">
       <c r="M35" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="AF35" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AG35" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="AH35" t="s">
         <v>27</v>
@@ -2711,13 +2708,13 @@
     </row>
     <row r="36" spans="10:34" x14ac:dyDescent="0.25">
       <c r="M36" s="4" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="AF36" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AG36" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="AH36" t="s">
         <v>27</v>
@@ -2725,35 +2722,35 @@
     </row>
     <row r="37" spans="10:34" x14ac:dyDescent="0.25">
       <c r="M37" s="4" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="AF37" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="AG37" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="38" spans="10:34" x14ac:dyDescent="0.25">
       <c r="M38" s="4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="AF38" t="s">
+        <v>63</v>
+      </c>
+      <c r="AG38" t="s">
         <v>65</v>
-      </c>
-      <c r="AG38" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="39" spans="10:34" x14ac:dyDescent="0.25">
       <c r="M39" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="AF39" t="s">
         <v>16</v>
       </c>
       <c r="AG39" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="AH39" t="s">
         <v>27</v>
@@ -2762,13 +2759,13 @@
     <row r="40" spans="10:34" x14ac:dyDescent="0.25">
       <c r="J40" s="6"/>
       <c r="M40" s="5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="AF40" t="s">
         <v>16</v>
       </c>
       <c r="AG40" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="AH40" t="s">
         <v>27</v>
@@ -2776,17 +2773,17 @@
     </row>
     <row r="41" spans="10:34" x14ac:dyDescent="0.25">
       <c r="M41" s="5" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="42" spans="10:34" x14ac:dyDescent="0.25">
       <c r="M42" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="43" spans="10:34" x14ac:dyDescent="0.25">
       <c r="M43" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="AE43" s="17" t="s">
         <v>36</v>
@@ -2796,15 +2793,15 @@
     </row>
     <row r="44" spans="10:34" x14ac:dyDescent="0.25">
       <c r="M44" s="5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="AE44" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="45" spans="10:34" x14ac:dyDescent="0.25">
       <c r="M45" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="AE45" t="s">
         <v>37</v>
@@ -2817,7 +2814,7 @@
     </row>
     <row r="47" spans="10:34" x14ac:dyDescent="0.25">
       <c r="M47" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="48" spans="10:34" x14ac:dyDescent="0.25">
@@ -2827,17 +2824,17 @@
     </row>
     <row r="49" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M49" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="50" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M50" s="5" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="51" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M51" s="5" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed timing error for 4th golden eye pair and added more details for wiring from M1 and M2
</commit_message>
<xml_diff>
--- a/choreo/SateliteDiagram.xlsx
+++ b/choreo/SateliteDiagram.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="15" windowWidth="29160" windowHeight="7500"/>
+    <workbookView xWindow="180" yWindow="15" windowWidth="29160" windowHeight="7500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="281">
   <si>
     <t>B1</t>
   </si>
@@ -80,12 +80,6 @@
     <t>SCAB</t>
   </si>
   <si>
-    <t>B5 shot 2) wired to M5</t>
-  </si>
-  <si>
-    <t>B6 shot 2) wired to M6</t>
-  </si>
-  <si>
     <t>CUTS</t>
   </si>
   <si>
@@ -1245,6 +1239,24 @@
   </si>
   <si>
     <t>12) silver palm</t>
+  </si>
+  <si>
+    <t>B5 shot 2) wired 1/2 way to M5</t>
+  </si>
+  <si>
+    <t>B6 shot 2) wired 1/2 way to M6</t>
+  </si>
+  <si>
+    <t>M1 shot 12) wired in lake to normal M1 horizontal position</t>
+  </si>
+  <si>
+    <t>M2 shot 11) wired in lake to normal M2 horizontal position</t>
+  </si>
+  <si>
+    <t>M1 shot 18) wired in lake to normal M1 horizontal position</t>
+  </si>
+  <si>
+    <t>M2 shot 18) wired in lake to normal M2 horizontal position</t>
   </si>
 </sst>
 </file>
@@ -1498,7 +1510,6 @@
     <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1509,6 +1520,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1821,8 +1833,8 @@
   </sheetPr>
   <dimension ref="A3:X52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="V41" sqref="V41"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1893,19 +1905,19 @@
       <c r="A4" s="4"/>
       <c r="C4" s="4"/>
       <c r="G4" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="L4" s="17" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="V4" s="4"/>
       <c r="X4" s="4"/>
@@ -1914,19 +1926,19 @@
       <c r="A5" s="5"/>
       <c r="C5" s="5"/>
       <c r="G5" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="L5" s="17" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="Q5" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="V5" s="5"/>
       <c r="X5" s="5"/>
@@ -1934,424 +1946,424 @@
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="C6" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="L6" s="17" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="Q6" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="R6" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="V6" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="X6" s="4"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="C7" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="Q7" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="R7" s="6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="V7" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="X7" s="5"/>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="C8" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>8</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>3</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="O8" s="2" t="s">
         <v>2</v>
       </c>
       <c r="Q8" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="R8" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="T8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="V8" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="X8" s="4"/>
     </row>
     <row r="9" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="28" t="s">
-        <v>178</v>
+      <c r="A9" s="27" t="s">
+        <v>176</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J9" s="3"/>
       <c r="L9" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="O9" s="3"/>
       <c r="Q9" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="R9" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="T9" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="V9" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="X9" s="28" t="s">
-        <v>178</v>
+        <v>63</v>
+      </c>
+      <c r="X9" s="27" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="10" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="27" t="s">
-        <v>275</v>
+      <c r="A10" s="26" t="s">
+        <v>273</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="L10" s="17" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="O10" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="Q10" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="R10" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="T10" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="V10" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="X10" s="27" t="s">
-        <v>275</v>
+        <v>64</v>
+      </c>
+      <c r="X10" s="26" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="11" spans="1:24" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="C11" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="O11" s="6" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="Q11" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="R11" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="T11" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="V11" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="X11" s="5"/>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="C12" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H12" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="O12" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="Q12" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="R12" s="9" t="s">
         <v>250</v>
       </c>
-      <c r="J12" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="L12" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="O12" s="6" t="s">
-        <v>236</v>
-      </c>
-      <c r="Q12" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="R12" s="9" t="s">
-        <v>252</v>
-      </c>
       <c r="T12" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="V12" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="X12" s="5"/>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="C13" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="J13" s="18" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O13" s="18" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="Q13" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="R13" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="T13" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="V13" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="X13" s="5"/>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="C14" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J14" s="18" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="O14" s="18" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="Q14" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="R14" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="T14" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="V14" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="X14" s="5"/>
     </row>
     <row r="15" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
-      <c r="C15" s="29" t="s">
-        <v>273</v>
+      <c r="C15" s="28" t="s">
+        <v>271</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="J15" s="18" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="L15" s="5" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="O15" s="18" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="Q15" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="R15" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="T15" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="V15" s="29" t="s">
-        <v>273</v>
+        <v>75</v>
+      </c>
+      <c r="V15" s="28" t="s">
+        <v>271</v>
       </c>
       <c r="X15" s="5"/>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="C16" s="5" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="J16" s="18" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="O16" s="18" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Q16" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="R16" s="10" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="T16" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="V16" s="5" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="X16" s="5"/>
     </row>
     <row r="17" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
-      <c r="C17" s="26" t="s">
-        <v>276</v>
+      <c r="C17" s="25" t="s">
+        <v>274</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="J17" s="18" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="L17" s="5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="O17" s="18" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="Q17" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="R17" s="6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="T17" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="V17" s="26" t="s">
-        <v>276</v>
+        <v>77</v>
+      </c>
+      <c r="V17" s="25" t="s">
+        <v>274</v>
       </c>
       <c r="X17" s="5"/>
     </row>
@@ -2359,31 +2371,31 @@
       <c r="A18" s="5"/>
       <c r="C18" s="5"/>
       <c r="E18" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="J18" s="18" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="L18" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="O18" s="18" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="Q18" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="R18" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="T18" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="V18" s="5"/>
       <c r="X18" s="5"/>
@@ -2392,31 +2404,31 @@
       <c r="A19" s="5"/>
       <c r="C19" s="5"/>
       <c r="E19" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="J19" s="18" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="O19" s="7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="Q19" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="R19" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="T19" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="V19" s="5"/>
       <c r="X19" s="5"/>
@@ -2425,31 +2437,31 @@
       <c r="A20" s="5"/>
       <c r="C20" s="5"/>
       <c r="E20" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="L20" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="O20" s="3" t="s">
-        <v>148</v>
+        <v>111</v>
+      </c>
+      <c r="O20" s="29" t="s">
+        <v>146</v>
       </c>
       <c r="Q20" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="R20" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="T20" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="V20" s="5"/>
       <c r="X20" s="5"/>
@@ -2458,31 +2470,31 @@
       <c r="A21" s="5"/>
       <c r="C21" s="5"/>
       <c r="E21" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="J21" s="3" t="s">
-        <v>112</v>
+        <v>132</v>
+      </c>
+      <c r="J21" s="29" t="s">
+        <v>110</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="O21" s="18" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="Q21" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="R21" s="12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="T21" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="V21" s="5"/>
       <c r="X21" s="5"/>
@@ -2491,31 +2503,31 @@
       <c r="A22" s="5"/>
       <c r="C22" s="5"/>
       <c r="E22" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J22" s="18" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="L22" s="8" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="O22" s="10" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="Q22" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="R22" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="T22" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="V22" s="5"/>
       <c r="X22" s="5"/>
@@ -2524,31 +2536,31 @@
       <c r="A23" s="5"/>
       <c r="C23" s="5"/>
       <c r="E23" s="10" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="J23" s="13" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="O23" s="13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="Q23" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="R23" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="T23" s="10" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="V23" s="5"/>
       <c r="X23" s="5"/>
@@ -2557,31 +2569,31 @@
       <c r="A24" s="5"/>
       <c r="C24" s="5"/>
       <c r="E24" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="J24" s="13" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="O24" s="13" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="Q24" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="R24" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="T24" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="V24" s="5"/>
       <c r="X24" s="5"/>
@@ -2590,31 +2602,31 @@
       <c r="A25" s="5"/>
       <c r="C25" s="5"/>
       <c r="E25" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="J25" s="13" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="O25" s="13" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="Q25" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="R25" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="T25" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="V25" s="5"/>
       <c r="X25" s="5"/>
@@ -2623,31 +2635,31 @@
       <c r="A26" s="5"/>
       <c r="C26" s="5"/>
       <c r="E26" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J26" s="13" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="L26" s="8" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="O26" s="13" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="Q26" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="R26" s="6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="T26" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="V26" s="5"/>
       <c r="X26" s="5"/>
@@ -2656,217 +2668,217 @@
       <c r="A27" s="5"/>
       <c r="C27" s="5"/>
       <c r="E27" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="J27" s="19" t="s">
-        <v>147</v>
+        <v>119</v>
+      </c>
+      <c r="J27" s="7" t="s">
+        <v>145</v>
       </c>
       <c r="L27" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="O27" s="19" t="s">
-        <v>147</v>
+        <v>155</v>
+      </c>
+      <c r="O27" s="7" t="s">
+        <v>145</v>
       </c>
       <c r="Q27" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="R27" s="6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="T27" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="V27" s="5"/>
       <c r="X27" s="5"/>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E28" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J28" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="M28" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="O28" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="T28" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E29" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J29" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="M29" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="O29" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="T29" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E30" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J30" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="M30" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="O30" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="T30" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E31" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="J31" s="22" t="s">
-        <v>101</v>
+        <v>90</v>
+      </c>
+      <c r="J31" s="21" t="s">
+        <v>99</v>
       </c>
       <c r="M31" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="O31" s="22" t="s">
-        <v>101</v>
+        <v>159</v>
+      </c>
+      <c r="O31" s="21" t="s">
+        <v>99</v>
       </c>
       <c r="T31" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E32" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="J32" s="23" t="s">
-        <v>268</v>
+        <v>91</v>
+      </c>
+      <c r="J32" s="22" t="s">
+        <v>266</v>
       </c>
       <c r="M32" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="O32" s="23" t="s">
-        <v>268</v>
+        <v>160</v>
+      </c>
+      <c r="O32" s="22" t="s">
+        <v>266</v>
       </c>
       <c r="T32" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="33" spans="10:15" x14ac:dyDescent="0.25">
       <c r="J33" s="6"/>
       <c r="M33" s="5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="O33" s="6"/>
     </row>
     <row r="34" spans="10:15" x14ac:dyDescent="0.25">
       <c r="J34" s="6"/>
       <c r="M34" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="O34" s="6"/>
     </row>
     <row r="35" spans="10:15" x14ac:dyDescent="0.25">
       <c r="M35" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="36" spans="10:15" x14ac:dyDescent="0.25">
       <c r="M36" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="37" spans="10:15" x14ac:dyDescent="0.25">
       <c r="M37" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="38" spans="10:15" x14ac:dyDescent="0.25">
       <c r="M38" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="39" spans="10:15" x14ac:dyDescent="0.25">
       <c r="M39" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="40" spans="10:15" x14ac:dyDescent="0.25">
       <c r="M40" s="5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="41" spans="10:15" x14ac:dyDescent="0.25">
       <c r="M41" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="42" spans="10:15" x14ac:dyDescent="0.25">
       <c r="M42" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="43" spans="10:15" x14ac:dyDescent="0.25">
       <c r="M43" s="5" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="44" spans="10:15" x14ac:dyDescent="0.25">
       <c r="M44" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="45" spans="10:15" x14ac:dyDescent="0.25">
       <c r="M45" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="46" spans="10:15" x14ac:dyDescent="0.25">
       <c r="M46" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="47" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="M47" s="24" t="s">
-        <v>176</v>
+      <c r="M47" s="23" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="48" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="M48" s="25" t="s">
-        <v>269</v>
+      <c r="M48" s="24" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="49" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M49" s="5" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="50" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M50" s="5" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="51" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M51" s="5" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="52" spans="13:13" x14ac:dyDescent="0.25">
@@ -2874,16 +2886,19 @@
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="5" scale="43" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup paperSize="5" scale="43" orientation="landscape" horizontalDpi="4294967293" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J43"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2898,7 +2913,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
@@ -2913,7 +2928,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>17</v>
@@ -2922,10 +2937,10 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -2936,19 +2951,19 @@
         <v>6</v>
       </c>
       <c r="F3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G3" t="s">
+        <v>185</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>187</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>189</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
       </c>
       <c r="J3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -2959,16 +2974,16 @@
         <v>4</v>
       </c>
       <c r="G4" t="s">
+        <v>186</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>188</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>190</v>
       </c>
       <c r="I4" t="s">
         <v>20</v>
       </c>
       <c r="J4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -2979,13 +2994,13 @@
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="J5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -2996,13 +3011,13 @@
         <v>6</v>
       </c>
       <c r="G6" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="J6" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -3013,13 +3028,13 @@
         <v>4</v>
       </c>
       <c r="G7" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -3030,13 +3045,13 @@
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="J8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -3047,16 +3062,16 @@
         <v>8</v>
       </c>
       <c r="F9" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G9" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="J9" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -3067,13 +3082,13 @@
         <v>10</v>
       </c>
       <c r="G10" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="J10" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -3084,13 +3099,13 @@
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="J11" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -3101,13 +3116,13 @@
         <v>8</v>
       </c>
       <c r="G12" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="J12" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -3118,50 +3133,50 @@
         <v>10</v>
       </c>
       <c r="G13" t="s">
+        <v>260</v>
+      </c>
+      <c r="H13" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="H13" s="3" t="s">
-        <v>264</v>
-      </c>
       <c r="J13" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>3</v>
       </c>
       <c r="G14" t="s">
+        <v>261</v>
+      </c>
+      <c r="H14" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="H14" s="3" t="s">
-        <v>265</v>
-      </c>
       <c r="J14" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="18" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>2</v>
       </c>
       <c r="F15" t="s">
+        <v>191</v>
+      </c>
+      <c r="G15" t="s">
+        <v>192</v>
+      </c>
+      <c r="H15" s="3" t="s">
         <v>193</v>
-      </c>
-      <c r="G15" t="s">
-        <v>194</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>195</v>
       </c>
       <c r="I15" t="s">
         <v>20</v>
@@ -3169,7 +3184,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>19</v>
@@ -3178,10 +3193,10 @@
         <v>8</v>
       </c>
       <c r="G16" t="s">
+        <v>192</v>
+      </c>
+      <c r="H16" s="3" t="s">
         <v>194</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>196</v>
       </c>
       <c r="I16" t="s">
         <v>20</v>
@@ -3195,10 +3210,10 @@
         <v>10</v>
       </c>
       <c r="G17" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>21</v>
+        <v>275</v>
       </c>
       <c r="I17" t="s">
         <v>20</v>
@@ -3212,10 +3227,10 @@
         <v>3</v>
       </c>
       <c r="G18" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>22</v>
+        <v>276</v>
       </c>
       <c r="I18" t="s">
         <v>20</v>
@@ -3229,21 +3244,21 @@
         <v>2</v>
       </c>
       <c r="F19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G19" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J19" t="s">
-        <v>197</v>
+        <v>277</v>
+      </c>
+      <c r="I19" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>13</v>
@@ -3252,53 +3267,47 @@
         <v>0</v>
       </c>
       <c r="G20" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J20" t="s">
-        <v>197</v>
+        <v>278</v>
+      </c>
+      <c r="I20" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="21" t="s">
+      <c r="B21" s="20" t="s">
         <v>13</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>3</v>
       </c>
       <c r="G21" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>198</v>
+        <v>23</v>
       </c>
       <c r="J21" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B22" s="21" t="s">
+      <c r="B22" s="20" t="s">
         <v>13</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F22" t="s">
-        <v>29</v>
-      </c>
       <c r="G22" t="s">
-        <v>209</v>
+        <v>26</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="I22" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="J22" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -3309,16 +3318,13 @@
         <v>9</v>
       </c>
       <c r="G23" t="s">
-        <v>210</v>
+        <v>26</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="I23" t="s">
-        <v>20</v>
+        <v>196</v>
       </c>
       <c r="J23" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -3328,140 +3334,149 @@
       <c r="C24" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="F24" t="s">
+        <v>27</v>
+      </c>
       <c r="G24" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="I24" t="s">
         <v>20</v>
       </c>
       <c r="J24" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G25" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="I25" t="s">
         <v>20</v>
       </c>
       <c r="J25" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B26" s="16"/>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
       <c r="E26" s="16"/>
       <c r="G26" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="I26" t="s">
         <v>20</v>
       </c>
       <c r="J26" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G27" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="I27" t="s">
         <v>20</v>
       </c>
       <c r="J27" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G28" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="I28" t="s">
         <v>20</v>
       </c>
       <c r="J28" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G29" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="I29" t="s">
         <v>20</v>
       </c>
       <c r="J29" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="20" t="s">
-        <v>230</v>
-      </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
+      <c r="A30" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="B30" s="19"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
       <c r="G30" t="s">
-        <v>14</v>
+        <v>211</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>217</v>
+        <v>246</v>
       </c>
       <c r="I30" t="s">
         <v>20</v>
       </c>
+      <c r="J30" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G31" t="s">
-        <v>14</v>
+        <v>212</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>218</v>
+        <v>247</v>
       </c>
       <c r="I31" t="s">
         <v>20</v>
       </c>
+      <c r="J31" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G32" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>219</v>
+        <v>279</v>
       </c>
       <c r="I32" t="s">
         <v>20</v>
@@ -3469,10 +3484,10 @@
     </row>
     <row r="33" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G33" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>220</v>
+        <v>280</v>
       </c>
       <c r="I33" t="s">
         <v>20</v>
@@ -3480,10 +3495,10 @@
     </row>
     <row r="34" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G34" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="I34" t="s">
         <v>20</v>
@@ -3491,10 +3506,10 @@
     </row>
     <row r="35" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G35" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="I35" t="s">
         <v>20</v>
@@ -3502,10 +3517,10 @@
     </row>
     <row r="36" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G36" t="s">
-        <v>31</v>
-      </c>
-      <c r="H36" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>217</v>
       </c>
       <c r="I36" t="s">
         <v>20</v>
@@ -3513,10 +3528,10 @@
     </row>
     <row r="37" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G37" t="s">
-        <v>31</v>
-      </c>
-      <c r="H37" s="4" t="s">
-        <v>34</v>
+        <v>28</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>218</v>
       </c>
       <c r="I37" t="s">
         <v>20</v>
@@ -3524,71 +3539,116 @@
     </row>
     <row r="38" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G38" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="J38" t="s">
-        <v>223</v>
+        <v>219</v>
+      </c>
+      <c r="I38" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="39" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G39" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="J39" t="s">
-        <v>223</v>
+        <v>220</v>
+      </c>
+      <c r="I39" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="40" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G40" t="s">
-        <v>15</v>
-      </c>
-      <c r="H40" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="J40" t="s">
-        <v>223</v>
+        <v>29</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I40" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="41" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G41" t="s">
-        <v>15</v>
-      </c>
-      <c r="H41" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="J41" t="s">
-        <v>223</v>
+        <v>29</v>
+      </c>
+      <c r="H41" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I41" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="42" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G42" t="s">
-        <v>15</v>
-      </c>
-      <c r="H42" s="4" t="s">
-        <v>226</v>
+        <v>33</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>222</v>
       </c>
       <c r="J42" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="43" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G43" t="s">
+        <v>33</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="J43" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="44" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G44" t="s">
         <v>15</v>
       </c>
-      <c r="H43" s="4" t="s">
+      <c r="H44" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="J44" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="45" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G45" t="s">
+        <v>15</v>
+      </c>
+      <c r="H45" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="J43" t="s">
-        <v>223</v>
+      <c r="J45" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="46" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G46" t="s">
+        <v>15</v>
+      </c>
+      <c r="H46" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="J46" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="47" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G47" t="s">
+        <v>15</v>
+      </c>
+      <c r="H47" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="J47" t="s">
+        <v>221</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="5" scale="70" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated cues and sats for colourful dahlia and remove vulcan for trip kaleids
</commit_message>
<xml_diff>
--- a/choreo/SateliteDiagram.xlsx
+++ b/choreo/SateliteDiagram.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="285">
   <si>
     <t>B1</t>
   </si>
@@ -119,9 +119,6 @@
     <t>golden rain willow</t>
   </si>
   <si>
-    <t>1) dragon spawn</t>
-  </si>
-  <si>
     <t>2) detonator 2</t>
   </si>
   <si>
@@ -625,9 +622,6 @@
     <t>lost together</t>
   </si>
   <si>
-    <t>_NONE_</t>
-  </si>
-  <si>
     <t>the oaf</t>
   </si>
   <si>
@@ -1257,13 +1251,50 @@
   </si>
   <si>
     <t>M2 shot 18) wired in lake to normal M2 horizontal position</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">1) colourful dahlia </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="3" tint="0.39997558519241921"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(pair)</t>
+    </r>
+  </si>
+  <si>
+    <t>colourful dahlia pair #1</t>
+  </si>
+  <si>
+    <t>B3 shot 1) tight V shape</t>
+  </si>
+  <si>
+    <t>colourful dahlia pair #2</t>
+  </si>
+  <si>
+    <t>B4 shot 1) tight V shape</t>
+  </si>
+  <si>
+    <t>91 shot kalied (triple)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1329,6 +1360,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="3" tint="0.39997558519241921"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1834,7 +1872,7 @@
   <dimension ref="A3:X52"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O27" sqref="O27"/>
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1905,19 +1943,19 @@
       <c r="A4" s="4"/>
       <c r="C4" s="4"/>
       <c r="G4" s="4" t="s">
-        <v>34</v>
+        <v>279</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L4" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>34</v>
+        <v>279</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="V4" s="4"/>
       <c r="X4" s="4"/>
@@ -1926,19 +1964,19 @@
       <c r="A5" s="5"/>
       <c r="C5" s="5"/>
       <c r="G5" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L5" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q5" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V5" s="5"/>
       <c r="X5" s="5"/>
@@ -1946,424 +1984,424 @@
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="C6" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L6" s="17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="Q6" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="R6" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="V6" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="X6" s="4"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="C7" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="Q7" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R7" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="V7" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="X7" s="5"/>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="C8" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>8</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>3</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="O8" s="2" t="s">
         <v>2</v>
       </c>
       <c r="Q8" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R8" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="T8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="V8" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="X8" s="4"/>
     </row>
     <row r="9" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="27" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J9" s="3"/>
       <c r="L9" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="O9" s="3"/>
       <c r="Q9" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="R9" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="T9" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="V9" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="X9" s="27" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="10" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="26" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L10" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="O10" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="Q10" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="R10" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="T10" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="V10" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="X10" s="26" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="11" spans="1:24" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="C11" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="O11" s="6" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="Q11" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="R11" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="T11" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="V11" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="X11" s="5"/>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="C12" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H12" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="O12" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="Q12" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="R12" s="9" t="s">
         <v>248</v>
       </c>
-      <c r="J12" s="6" t="s">
-        <v>233</v>
-      </c>
-      <c r="L12" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="O12" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="Q12" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="R12" s="9" t="s">
-        <v>250</v>
-      </c>
       <c r="T12" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="V12" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="X12" s="5"/>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="C13" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J13" s="18" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="O13" s="18" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="Q13" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R13" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="T13" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="V13" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="X13" s="5"/>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="C14" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J14" s="18" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O14" s="18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="Q14" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="R14" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T14" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="V14" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="X14" s="5"/>
     </row>
     <row r="15" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="C15" s="28" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J15" s="18" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L15" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O15" s="18" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="Q15" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="R15" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="T15" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="V15" s="28" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="X15" s="5"/>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="C16" s="5" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="J16" s="18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="O16" s="18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q16" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="R16" s="10" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="T16" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="V16" s="5" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="X16" s="5"/>
     </row>
     <row r="17" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
       <c r="C17" s="25" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J17" s="18" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L17" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="O17" s="18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Q17" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="R17" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="T17" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="V17" s="25" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="X17" s="5"/>
     </row>
@@ -2371,31 +2409,31 @@
       <c r="A18" s="5"/>
       <c r="C18" s="5"/>
       <c r="E18" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J18" s="18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L18" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="O18" s="18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Q18" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R18" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="T18" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="V18" s="5"/>
       <c r="X18" s="5"/>
@@ -2404,31 +2442,31 @@
       <c r="A19" s="5"/>
       <c r="C19" s="5"/>
       <c r="E19" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J19" s="18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="O19" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="Q19" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="R19" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="T19" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="V19" s="5"/>
       <c r="X19" s="5"/>
@@ -2437,31 +2475,31 @@
       <c r="A20" s="5"/>
       <c r="C20" s="5"/>
       <c r="E20" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L20" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="O20" s="29" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="Q20" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="R20" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="T20" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="V20" s="5"/>
       <c r="X20" s="5"/>
@@ -2470,31 +2508,31 @@
       <c r="A21" s="5"/>
       <c r="C21" s="5"/>
       <c r="E21" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J21" s="29" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="O21" s="18" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="Q21" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="R21" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="T21" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="V21" s="5"/>
       <c r="X21" s="5"/>
@@ -2503,31 +2541,31 @@
       <c r="A22" s="5"/>
       <c r="C22" s="5"/>
       <c r="E22" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J22" s="18" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="L22" s="8" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="O22" s="10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="Q22" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="R22" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="T22" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="V22" s="5"/>
       <c r="X22" s="5"/>
@@ -2536,31 +2574,31 @@
       <c r="A23" s="5"/>
       <c r="C23" s="5"/>
       <c r="E23" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J23" s="13" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="O23" s="13" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="Q23" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="R23" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="T23" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="V23" s="5"/>
       <c r="X23" s="5"/>
@@ -2569,31 +2607,31 @@
       <c r="A24" s="5"/>
       <c r="C24" s="5"/>
       <c r="E24" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J24" s="13" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="O24" s="13" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="Q24" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="R24" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="T24" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="V24" s="5"/>
       <c r="X24" s="5"/>
@@ -2602,31 +2640,31 @@
       <c r="A25" s="5"/>
       <c r="C25" s="5"/>
       <c r="E25" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J25" s="13" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="O25" s="13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="Q25" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="R25" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="T25" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="V25" s="5"/>
       <c r="X25" s="5"/>
@@ -2635,31 +2673,31 @@
       <c r="A26" s="5"/>
       <c r="C26" s="5"/>
       <c r="E26" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J26" s="13" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="L26" s="8" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="O26" s="13" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="Q26" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="R26" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="T26" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="V26" s="5"/>
       <c r="X26" s="5"/>
@@ -2668,217 +2706,217 @@
       <c r="A27" s="5"/>
       <c r="C27" s="5"/>
       <c r="E27" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J27" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="L27" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="O27" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="Q27" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="R27" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="T27" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="V27" s="5"/>
       <c r="X27" s="5"/>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E28" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J28" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M28" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O28" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="T28" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E29" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J29" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M29" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="O29" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="T29" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E30" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J30" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M30" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="O30" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="T30" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E31" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J31" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M31" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="O31" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="T31" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E32" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J32" s="22" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="M32" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="O32" s="22" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="T32" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="10:15" x14ac:dyDescent="0.25">
       <c r="J33" s="6"/>
       <c r="M33" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O33" s="6"/>
     </row>
     <row r="34" spans="10:15" x14ac:dyDescent="0.25">
       <c r="J34" s="6"/>
       <c r="M34" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O34" s="6"/>
     </row>
     <row r="35" spans="10:15" x14ac:dyDescent="0.25">
       <c r="M35" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="36" spans="10:15" x14ac:dyDescent="0.25">
       <c r="M36" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="37" spans="10:15" x14ac:dyDescent="0.25">
       <c r="M37" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="38" spans="10:15" x14ac:dyDescent="0.25">
       <c r="M38" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="39" spans="10:15" x14ac:dyDescent="0.25">
       <c r="M39" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="40" spans="10:15" x14ac:dyDescent="0.25">
       <c r="M40" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="41" spans="10:15" x14ac:dyDescent="0.25">
       <c r="M41" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="42" spans="10:15" x14ac:dyDescent="0.25">
       <c r="M42" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="43" spans="10:15" x14ac:dyDescent="0.25">
       <c r="M43" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="44" spans="10:15" x14ac:dyDescent="0.25">
       <c r="M44" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="45" spans="10:15" x14ac:dyDescent="0.25">
       <c r="M45" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="46" spans="10:15" x14ac:dyDescent="0.25">
       <c r="M46" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="47" spans="10:15" x14ac:dyDescent="0.25">
       <c r="M47" s="23" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="48" spans="10:15" x14ac:dyDescent="0.25">
       <c r="M48" s="24" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="49" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M49" s="5" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="50" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M50" s="5" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="51" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M51" s="5" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="52" spans="13:13" x14ac:dyDescent="0.25">
@@ -2895,10 +2933,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J47"/>
+  <dimension ref="A1:J50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2913,7 +2951,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
@@ -2928,7 +2966,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>17</v>
@@ -2937,10 +2975,16 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G2" t="s">
-        <v>190</v>
+        <v>280</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="J2" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -2950,20 +2994,14 @@
       <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F3" t="s">
-        <v>184</v>
-      </c>
       <c r="G3" t="s">
-        <v>185</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="I3" t="s">
-        <v>20</v>
+        <v>282</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>283</v>
       </c>
       <c r="J3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -2973,17 +3011,20 @@
       <c r="C4" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="F4" t="s">
+        <v>183</v>
+      </c>
       <c r="G4" t="s">
+        <v>184</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>186</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>188</v>
       </c>
       <c r="I4" t="s">
         <v>20</v>
       </c>
       <c r="J4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -2994,13 +3035,16 @@
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>230</v>
+        <v>185</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>236</v>
+        <v>187</v>
+      </c>
+      <c r="I5" t="s">
+        <v>20</v>
       </c>
       <c r="J5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -3011,13 +3055,13 @@
         <v>6</v>
       </c>
       <c r="G6" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="J6" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -3028,13 +3072,13 @@
         <v>4</v>
       </c>
       <c r="G7" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J7" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -3045,13 +3089,13 @@
         <v>0</v>
       </c>
       <c r="G8" t="s">
+        <v>228</v>
+      </c>
+      <c r="H8" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="H8" s="3" t="s">
-        <v>239</v>
-      </c>
       <c r="J8" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -3061,17 +3105,14 @@
       <c r="C9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F9" t="s">
-        <v>189</v>
-      </c>
       <c r="G9" t="s">
-        <v>251</v>
+        <v>233</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>254</v>
+        <v>237</v>
       </c>
       <c r="J9" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -3082,13 +3123,7 @@
         <v>10</v>
       </c>
       <c r="G10" t="s">
-        <v>252</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="J10" t="s">
-        <v>195</v>
+        <v>284</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -3099,13 +3134,7 @@
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>253</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="J11" t="s">
-        <v>195</v>
+        <v>284</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -3115,14 +3144,17 @@
       <c r="C12" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="F12" t="s">
+        <v>188</v>
+      </c>
       <c r="G12" t="s">
-        <v>258</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>259</v>
+        <v>249</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>252</v>
       </c>
       <c r="J12" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -3133,58 +3165,55 @@
         <v>10</v>
       </c>
       <c r="G13" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="J13" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>114</v>
+      </c>
+      <c r="B14" s="18" t="s">
         <v>115</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>116</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>3</v>
       </c>
       <c r="G14" t="s">
-        <v>261</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>263</v>
+        <v>251</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>254</v>
       </c>
       <c r="J14" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F15" t="s">
-        <v>191</v>
-      </c>
       <c r="G15" t="s">
-        <v>192</v>
-      </c>
-      <c r="H15" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="J15" t="s">
         <v>193</v>
-      </c>
-      <c r="I15" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>19</v>
@@ -3193,13 +3222,13 @@
         <v>8</v>
       </c>
       <c r="G16" t="s">
-        <v>192</v>
+        <v>258</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="I16" t="s">
-        <v>20</v>
+        <v>260</v>
+      </c>
+      <c r="J16" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -3210,13 +3239,13 @@
         <v>10</v>
       </c>
       <c r="G17" t="s">
-        <v>198</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>275</v>
-      </c>
-      <c r="I17" t="s">
-        <v>20</v>
+        <v>259</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="J17" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -3226,11 +3255,14 @@
       <c r="C18" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="F18" t="s">
+        <v>189</v>
+      </c>
       <c r="G18" t="s">
-        <v>198</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>276</v>
+        <v>190</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>191</v>
       </c>
       <c r="I18" t="s">
         <v>20</v>
@@ -3243,14 +3275,11 @@
       <c r="C19" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F19" t="s">
-        <v>25</v>
-      </c>
       <c r="G19" t="s">
-        <v>19</v>
+        <v>190</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>277</v>
+        <v>192</v>
       </c>
       <c r="I19" t="s">
         <v>20</v>
@@ -3267,10 +3296,10 @@
         <v>0</v>
       </c>
       <c r="G20" t="s">
-        <v>19</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>278</v>
+        <v>196</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>273</v>
       </c>
       <c r="I20" t="s">
         <v>20</v>
@@ -3284,13 +3313,13 @@
         <v>3</v>
       </c>
       <c r="G21" t="s">
-        <v>26</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J21" t="s">
-        <v>195</v>
+        <v>196</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="I21" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -3300,14 +3329,17 @@
       <c r="C22" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="F22" t="s">
+        <v>25</v>
+      </c>
       <c r="G22" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="J22" t="s">
-        <v>195</v>
+        <v>275</v>
+      </c>
+      <c r="I22" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -3318,13 +3350,13 @@
         <v>9</v>
       </c>
       <c r="G23" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="J23" t="s">
-        <v>195</v>
+        <v>276</v>
+      </c>
+      <c r="I23" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -3334,34 +3366,25 @@
       <c r="C24" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F24" t="s">
-        <v>27</v>
-      </c>
       <c r="G24" t="s">
-        <v>207</v>
+        <v>26</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="I24" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="J24" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G25" t="s">
-        <v>208</v>
+        <v>26</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="I25" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="J25" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -3373,33 +3396,33 @@
       <c r="D26" s="16"/>
       <c r="E26" s="16"/>
       <c r="G26" t="s">
-        <v>209</v>
+        <v>26</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="I26" t="s">
-        <v>20</v>
+        <v>194</v>
       </c>
       <c r="J26" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>117</v>
+        <v>116</v>
+      </c>
+      <c r="F27" t="s">
+        <v>27</v>
       </c>
       <c r="G27" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="I27" t="s">
         <v>20</v>
       </c>
       <c r="J27" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -3407,109 +3430,118 @@
         <v>22</v>
       </c>
       <c r="G28" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="I28" t="s">
         <v>20</v>
       </c>
       <c r="J28" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G29" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="I29" t="s">
         <v>20</v>
       </c>
       <c r="J29" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="19" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B30" s="19"/>
       <c r="C30" s="19"/>
       <c r="D30" s="19"/>
       <c r="E30" s="19"/>
       <c r="G30" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="I30" t="s">
         <v>20</v>
       </c>
       <c r="J30" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="G31" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="I31" t="s">
         <v>20</v>
       </c>
       <c r="J31" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G32" t="s">
-        <v>13</v>
+        <v>211</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>279</v>
+        <v>243</v>
       </c>
       <c r="I32" t="s">
         <v>20</v>
       </c>
+      <c r="J32" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="33" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G33" t="s">
-        <v>13</v>
+        <v>209</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>280</v>
+        <v>244</v>
       </c>
       <c r="I33" t="s">
         <v>20</v>
       </c>
+      <c r="J33" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="34" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G34" t="s">
-        <v>14</v>
+        <v>210</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>215</v>
+        <v>245</v>
       </c>
       <c r="I34" t="s">
         <v>20</v>
       </c>
+      <c r="J34" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="35" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G35" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>216</v>
+        <v>277</v>
       </c>
       <c r="I35" t="s">
         <v>20</v>
@@ -3517,10 +3549,10 @@
     </row>
     <row r="36" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G36" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>217</v>
+        <v>278</v>
       </c>
       <c r="I36" t="s">
         <v>20</v>
@@ -3528,10 +3560,10 @@
     </row>
     <row r="37" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G37" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="I37" t="s">
         <v>20</v>
@@ -3539,10 +3571,10 @@
     </row>
     <row r="38" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G38" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="I38" t="s">
         <v>20</v>
@@ -3550,10 +3582,10 @@
     </row>
     <row r="39" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G39" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="I39" t="s">
         <v>20</v>
@@ -3561,10 +3593,10 @@
     </row>
     <row r="40" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G40" t="s">
-        <v>29</v>
-      </c>
-      <c r="H40" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>216</v>
       </c>
       <c r="I40" t="s">
         <v>20</v>
@@ -3572,10 +3604,10 @@
     </row>
     <row r="41" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G41" t="s">
-        <v>29</v>
-      </c>
-      <c r="H41" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>217</v>
       </c>
       <c r="I41" t="s">
         <v>20</v>
@@ -3583,68 +3615,101 @@
     </row>
     <row r="42" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G42" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="J42" t="s">
-        <v>221</v>
+        <v>218</v>
+      </c>
+      <c r="I42" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="43" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G43" t="s">
-        <v>33</v>
-      </c>
-      <c r="H43" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="J43" t="s">
-        <v>221</v>
+        <v>29</v>
+      </c>
+      <c r="H43" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I43" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="44" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G44" t="s">
-        <v>15</v>
-      </c>
-      <c r="H44" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="J44" t="s">
-        <v>221</v>
+        <v>29</v>
+      </c>
+      <c r="H44" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I44" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="45" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G45" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="J45" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="46" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G46" t="s">
-        <v>15</v>
-      </c>
-      <c r="H46" s="4" t="s">
-        <v>224</v>
+        <v>33</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>221</v>
       </c>
       <c r="J46" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="47" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G47" t="s">
         <v>15</v>
       </c>
-      <c r="H47" s="4" t="s">
+      <c r="H47" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="J47" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="48" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G48" t="s">
+        <v>15</v>
+      </c>
+      <c r="H48" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="J47" t="s">
-        <v>221</v>
+      <c r="J48" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="49" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G49" t="s">
+        <v>15</v>
+      </c>
+      <c r="H49" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="J49" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="50" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G50" t="s">
+        <v>15</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="J50" t="s">
+        <v>219</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed wrong cue time in free world for Milan2017.kfb and on the cue chart; updated noted in sat diagrams;  updated vid projects.  still need one more fix pass
</commit_message>
<xml_diff>
--- a/choreo/SateliteDiagram.xlsx
+++ b/choreo/SateliteDiagram.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1096" uniqueCount="294">
   <si>
     <t>B1</t>
   </si>
@@ -393,9 +393,6 @@
     <t>24) Executioner</t>
   </si>
   <si>
-    <t>3) multi coloured peoni</t>
-  </si>
-  <si>
     <t>4) CDC-9393</t>
   </si>
   <si>
@@ -822,30 +819,9 @@
     </r>
   </si>
   <si>
-    <t>golden eye pair #1a</t>
-  </si>
-  <si>
-    <t>golden eye pair #1b</t>
-  </si>
-  <si>
-    <t>golden eye pair #2a</t>
-  </si>
-  <si>
-    <t>golden eye pair #3a</t>
-  </si>
-  <si>
-    <t>golden eye pair #4a</t>
-  </si>
-  <si>
     <t>golden eye pair #4b</t>
   </si>
   <si>
-    <t>golden eye pair #3b</t>
-  </si>
-  <si>
-    <t>golden eye pair #2b</t>
-  </si>
-  <si>
     <t>M1 shot 19) wired to 3's</t>
   </si>
   <si>
@@ -1288,6 +1264,76 @@
   </si>
   <si>
     <t>91 shot kalied (triple)</t>
+  </si>
+  <si>
+    <t>PAIRED FROM SINGLE CUE TO DIFFERENT LOCATIONS</t>
+  </si>
+  <si>
+    <t>B6 shot 10) - showstopper to extreme outside B6 and '007' to M6</t>
+  </si>
+  <si>
+    <t>B5 shot 10) - showstopper to extreme outside B5 and '007' to M5</t>
+  </si>
+  <si>
+    <t>B5 shot 12) - silver palm at an angle and golden rain wired to extreme outside B5</t>
+  </si>
+  <si>
+    <t>B6 shot 12) - silver palm at an angle and golden rain wired to extreme outside B6</t>
+  </si>
+  <si>
+    <t>B1 shot 20) - blistering cactus to lake and mines to front on lawn</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3) 91 shot kalied</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="3" tint="0.39997558519241921"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (triple)</t>
+    </r>
+  </si>
+  <si>
+    <t>M3 shot 3)   angled outward fan</t>
+  </si>
+  <si>
+    <t>M4 shot 3)   angled outward fan</t>
+  </si>
+  <si>
+    <t>sub zero pair #1a</t>
+  </si>
+  <si>
+    <t>sub zero pair #1b</t>
+  </si>
+  <si>
+    <t>sub zero pair #2a</t>
+  </si>
+  <si>
+    <t>sub zero pair #2b</t>
+  </si>
+  <si>
+    <t>sub zero pair #3a</t>
+  </si>
+  <si>
+    <t>sub zero pair #3b</t>
+  </si>
+  <si>
+    <t>sub zero pair #4a</t>
+  </si>
+  <si>
+    <t>sub zero pair #4b</t>
   </si>
 </sst>
 </file>
@@ -1372,7 +1418,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1433,6 +1479,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39994506668294322"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1528,7 +1586,7 @@
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1559,6 +1617,8 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1872,7 +1932,7 @@
   <dimension ref="A3:X52"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1943,7 +2003,7 @@
       <c r="A4" s="4"/>
       <c r="C4" s="4"/>
       <c r="G4" s="4" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>57</v>
@@ -1952,7 +2012,7 @@
         <v>100</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="R4" s="3" t="s">
         <v>57</v>
@@ -1990,7 +2050,7 @@
         <v>35</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>119</v>
+        <v>283</v>
       </c>
       <c r="L6" s="17" t="s">
         <v>102</v>
@@ -1999,7 +2059,7 @@
         <v>35</v>
       </c>
       <c r="R6" s="6" t="s">
-        <v>119</v>
+        <v>283</v>
       </c>
       <c r="V6" s="4" t="s">
         <v>59</v>
@@ -2015,7 +2075,7 @@
         <v>36</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L7" s="4" t="s">
         <v>103</v>
@@ -2024,7 +2084,7 @@
         <v>36</v>
       </c>
       <c r="R7" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="V7" s="11" t="s">
         <v>60</v>
@@ -2043,7 +2103,7 @@
         <v>37</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>3</v>
@@ -2058,7 +2118,7 @@
         <v>37</v>
       </c>
       <c r="R8" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="T8" s="2" t="s">
         <v>10</v>
@@ -2070,7 +2130,7 @@
     </row>
     <row r="9" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="27" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>62</v>
@@ -2102,12 +2162,12 @@
         <v>62</v>
       </c>
       <c r="X9" s="27" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="10" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="26" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>63</v>
@@ -2119,7 +2179,7 @@
         <v>39</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J10" s="7" t="s">
         <v>92</v>
@@ -2134,7 +2194,7 @@
         <v>39</v>
       </c>
       <c r="R10" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="T10" s="12" t="s">
         <v>91</v>
@@ -2143,7 +2203,7 @@
         <v>63</v>
       </c>
       <c r="X10" s="26" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
     </row>
     <row r="11" spans="1:24" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -2158,22 +2218,22 @@
         <v>40</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="L11" s="5" t="s">
         <v>107</v>
       </c>
       <c r="O11" s="6" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="Q11" s="5" t="s">
         <v>40</v>
       </c>
       <c r="R11" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="T11" s="6" t="s">
         <v>70</v>
@@ -2195,22 +2255,22 @@
         <v>41</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="L12" s="5" t="s">
         <v>108</v>
       </c>
       <c r="O12" s="6" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="Q12" s="4" t="s">
         <v>41</v>
       </c>
       <c r="R12" s="9" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="T12" s="6" t="s">
         <v>71</v>
@@ -2232,22 +2292,22 @@
         <v>42</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J13" s="18" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="L13" s="5" t="s">
         <v>94</v>
       </c>
       <c r="O13" s="18" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="Q13" s="4" t="s">
         <v>42</v>
       </c>
       <c r="R13" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="T13" s="3" t="s">
         <v>72</v>
@@ -2269,22 +2329,22 @@
         <v>43</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J14" s="18" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="O14" s="18" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="Q14" s="4" t="s">
         <v>43</v>
       </c>
       <c r="R14" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="T14" s="3" t="s">
         <v>73</v>
@@ -2297,7 +2357,7 @@
     <row r="15" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="C15" s="28" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>74</v>
@@ -2306,35 +2366,35 @@
         <v>44</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J15" s="18" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L15" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="O15" s="18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="Q15" s="4" t="s">
         <v>44</v>
       </c>
       <c r="R15" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T15" s="3" t="s">
         <v>74</v>
       </c>
       <c r="V15" s="28" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="X15" s="5"/>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="C16" s="5" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>75</v>
@@ -2343,35 +2403,35 @@
         <v>45</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="J16" s="18" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O16" s="18" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q16" s="4" t="s">
         <v>45</v>
       </c>
       <c r="R16" s="10" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="T16" s="3" t="s">
         <v>75</v>
       </c>
       <c r="V16" s="5" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="X16" s="5"/>
     </row>
     <row r="17" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
       <c r="C17" s="25" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>76</v>
@@ -2380,13 +2440,13 @@
         <v>46</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J17" s="18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L17" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O17" s="18" t="s">
         <v>93</v>
@@ -2395,13 +2455,13 @@
         <v>46</v>
       </c>
       <c r="R17" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="T17" s="6" t="s">
         <v>76</v>
       </c>
       <c r="V17" s="25" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="X17" s="5"/>
     </row>
@@ -2415,22 +2475,22 @@
         <v>47</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J18" s="18" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L18" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="O18" s="18" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q18" s="4" t="s">
         <v>47</v>
       </c>
       <c r="R18" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="T18" s="6" t="s">
         <v>77</v>
@@ -2448,22 +2508,22 @@
         <v>48</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J19" s="18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="O19" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="Q19" s="5" t="s">
         <v>48</v>
       </c>
       <c r="R19" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="T19" s="6" t="s">
         <v>78</v>
@@ -2475,31 +2535,31 @@
       <c r="A20" s="5"/>
       <c r="C20" s="5"/>
       <c r="E20" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>49</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L20" s="5" t="s">
         <v>110</v>
       </c>
       <c r="O20" s="29" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="Q20" s="5" t="s">
         <v>49</v>
       </c>
       <c r="R20" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="T20" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="V20" s="5"/>
       <c r="X20" s="5"/>
@@ -2514,22 +2574,22 @@
         <v>50</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J21" s="29" t="s">
         <v>109</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="O21" s="18" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="Q21" s="4" t="s">
         <v>50</v>
       </c>
       <c r="R21" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="T21" s="3" t="s">
         <v>79</v>
@@ -2550,13 +2610,13 @@
         <v>51</v>
       </c>
       <c r="J22" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L22" s="8" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="O22" s="10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="Q22" s="4" t="s">
         <v>51</v>
@@ -2580,22 +2640,22 @@
         <v>52</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J23" s="13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="O23" s="13" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="Q23" s="5" t="s">
         <v>52</v>
       </c>
       <c r="R23" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="T23" s="10" t="s">
         <v>81</v>
@@ -2613,22 +2673,22 @@
         <v>53</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J24" s="13" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L24" s="4" t="s">
         <v>87</v>
       </c>
       <c r="O24" s="13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="Q24" s="5" t="s">
         <v>53</v>
       </c>
       <c r="R24" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="T24" s="3" t="s">
         <v>82</v>
@@ -2646,22 +2706,22 @@
         <v>54</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J25" s="13" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="O25" s="13" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="Q25" s="5" t="s">
         <v>54</v>
       </c>
       <c r="R25" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="T25" s="3" t="s">
         <v>83</v>
@@ -2679,22 +2739,22 @@
         <v>55</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J26" s="13" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="L26" s="8" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="O26" s="13" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="Q26" s="5" t="s">
         <v>55</v>
       </c>
       <c r="R26" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="T26" s="3" t="s">
         <v>84</v>
@@ -2715,13 +2775,13 @@
         <v>118</v>
       </c>
       <c r="J27" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="L27" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="O27" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="Q27" s="5" t="s">
         <v>56</v>
@@ -2743,7 +2803,7 @@
         <v>95</v>
       </c>
       <c r="M28" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="O28" s="7" t="s">
         <v>95</v>
@@ -2760,7 +2820,7 @@
         <v>96</v>
       </c>
       <c r="M29" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O29" s="7" t="s">
         <v>96</v>
@@ -2777,7 +2837,7 @@
         <v>97</v>
       </c>
       <c r="M30" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="O30" s="7" t="s">
         <v>97</v>
@@ -2794,7 +2854,7 @@
         <v>98</v>
       </c>
       <c r="M31" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="O31" s="21" t="s">
         <v>98</v>
@@ -2808,13 +2868,13 @@
         <v>90</v>
       </c>
       <c r="J32" s="22" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="M32" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="O32" s="22" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="T32" s="6" t="s">
         <v>90</v>
@@ -2823,35 +2883,35 @@
     <row r="33" spans="10:15" x14ac:dyDescent="0.25">
       <c r="J33" s="6"/>
       <c r="M33" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="O33" s="6"/>
     </row>
     <row r="34" spans="10:15" x14ac:dyDescent="0.25">
       <c r="J34" s="6"/>
       <c r="M34" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O34" s="6"/>
     </row>
     <row r="35" spans="10:15" x14ac:dyDescent="0.25">
       <c r="M35" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="36" spans="10:15" x14ac:dyDescent="0.25">
       <c r="M36" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="37" spans="10:15" x14ac:dyDescent="0.25">
       <c r="M37" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="38" spans="10:15" x14ac:dyDescent="0.25">
       <c r="M38" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="39" spans="10:15" x14ac:dyDescent="0.25">
@@ -2861,62 +2921,62 @@
     </row>
     <row r="40" spans="10:15" x14ac:dyDescent="0.25">
       <c r="M40" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="41" spans="10:15" x14ac:dyDescent="0.25">
       <c r="M41" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="42" spans="10:15" x14ac:dyDescent="0.25">
       <c r="M42" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="43" spans="10:15" x14ac:dyDescent="0.25">
       <c r="M43" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="44" spans="10:15" x14ac:dyDescent="0.25">
       <c r="M44" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="45" spans="10:15" x14ac:dyDescent="0.25">
       <c r="M45" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="46" spans="10:15" x14ac:dyDescent="0.25">
       <c r="M46" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="47" spans="10:15" x14ac:dyDescent="0.25">
       <c r="M47" s="23" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="48" spans="10:15" x14ac:dyDescent="0.25">
       <c r="M48" s="24" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
     </row>
     <row r="49" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M49" s="5" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
     </row>
     <row r="50" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M50" s="5" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
     </row>
     <row r="51" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M51" s="5" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
     </row>
     <row r="52" spans="13:13" x14ac:dyDescent="0.25">
@@ -2935,8 +2995,8 @@
   </sheetPr>
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2975,16 +3035,16 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G2" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="J2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -2995,13 +3055,13 @@
         <v>6</v>
       </c>
       <c r="G3" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="J3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -3012,19 +3072,19 @@
         <v>4</v>
       </c>
       <c r="F4" t="s">
+        <v>182</v>
+      </c>
+      <c r="G4" t="s">
         <v>183</v>
       </c>
-      <c r="G4" t="s">
-        <v>184</v>
-      </c>
       <c r="H4" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I4" t="s">
         <v>20</v>
       </c>
       <c r="J4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -3035,16 +3095,16 @@
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I5" t="s">
         <v>20</v>
       </c>
       <c r="J5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -3055,13 +3115,13 @@
         <v>6</v>
       </c>
       <c r="G6" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="J6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -3072,13 +3132,13 @@
         <v>4</v>
       </c>
       <c r="G7" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="J7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -3089,13 +3149,13 @@
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="J8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -3106,13 +3166,13 @@
         <v>8</v>
       </c>
       <c r="G9" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="J9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -3123,7 +3183,13 @@
         <v>10</v>
       </c>
       <c r="G10" t="s">
+        <v>276</v>
+      </c>
+      <c r="H10" s="3" t="s">
         <v>284</v>
+      </c>
+      <c r="J10" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -3134,7 +3200,13 @@
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>284</v>
+        <v>276</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="J11" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -3145,16 +3217,16 @@
         <v>8</v>
       </c>
       <c r="F12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G12" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="J12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -3165,13 +3237,13 @@
         <v>10</v>
       </c>
       <c r="G13" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="J13" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -3185,13 +3257,13 @@
         <v>3</v>
       </c>
       <c r="G14" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="J14" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -3202,13 +3274,13 @@
         <v>2</v>
       </c>
       <c r="G15" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="J15" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -3222,13 +3294,13 @@
         <v>8</v>
       </c>
       <c r="G16" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="J16" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -3239,13 +3311,13 @@
         <v>10</v>
       </c>
       <c r="G17" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="J17" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -3256,13 +3328,13 @@
         <v>3</v>
       </c>
       <c r="F18" t="s">
+        <v>188</v>
+      </c>
+      <c r="G18" t="s">
         <v>189</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" s="3" t="s">
         <v>190</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>191</v>
       </c>
       <c r="I18" t="s">
         <v>20</v>
@@ -3276,10 +3348,10 @@
         <v>2</v>
       </c>
       <c r="G19" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I19" t="s">
         <v>20</v>
@@ -3296,10 +3368,10 @@
         <v>0</v>
       </c>
       <c r="G20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="I20" t="s">
         <v>20</v>
@@ -3313,10 +3385,10 @@
         <v>3</v>
       </c>
       <c r="G21" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="I21" t="s">
         <v>20</v>
@@ -3336,7 +3408,7 @@
         <v>19</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="I22" t="s">
         <v>20</v>
@@ -3353,7 +3425,7 @@
         <v>19</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="I23" t="s">
         <v>20</v>
@@ -3373,7 +3445,7 @@
         <v>23</v>
       </c>
       <c r="J24" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -3384,7 +3456,7 @@
         <v>24</v>
       </c>
       <c r="J25" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -3399,10 +3471,10 @@
         <v>26</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J26" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -3413,16 +3485,16 @@
         <v>27</v>
       </c>
       <c r="G27" t="s">
-        <v>205</v>
+        <v>286</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="I27" t="s">
         <v>20</v>
       </c>
       <c r="J27" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -3430,201 +3502,243 @@
         <v>22</v>
       </c>
       <c r="G28" t="s">
-        <v>206</v>
+        <v>287</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="I28" t="s">
         <v>20</v>
       </c>
       <c r="J28" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G29" t="s">
-        <v>207</v>
+        <v>288</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="I29" t="s">
         <v>20</v>
       </c>
       <c r="J29" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="19" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="B30" s="19"/>
       <c r="C30" s="19"/>
       <c r="D30" s="19"/>
       <c r="E30" s="19"/>
       <c r="G30" t="s">
-        <v>212</v>
+        <v>289</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="I30" t="s">
         <v>20</v>
       </c>
       <c r="J30" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="G31" t="s">
-        <v>208</v>
+        <v>290</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="I31" t="s">
         <v>20</v>
       </c>
       <c r="J31" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G32" t="s">
-        <v>211</v>
+        <v>291</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="I32" t="s">
         <v>20</v>
       </c>
       <c r="J32" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="33" spans="7:10" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="30" t="s">
+        <v>277</v>
+      </c>
+      <c r="B33" s="30"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="30"/>
       <c r="G33" t="s">
-        <v>209</v>
+        <v>292</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="I33" t="s">
         <v>20</v>
       </c>
       <c r="J33" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="34" spans="7:10" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="31" t="s">
+        <v>282</v>
+      </c>
+      <c r="B34" s="31"/>
+      <c r="C34" s="31"/>
+      <c r="D34" s="31"/>
+      <c r="E34" s="31"/>
       <c r="G34" t="s">
-        <v>210</v>
+        <v>293</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="I34" t="s">
         <v>20</v>
       </c>
       <c r="J34" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="35" spans="7:10" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="31" t="s">
+        <v>279</v>
+      </c>
+      <c r="B35" s="31"/>
+      <c r="C35" s="31"/>
+      <c r="D35" s="31"/>
+      <c r="E35" s="31"/>
       <c r="G35" t="s">
         <v>13</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I35" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="7:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="31" t="s">
+        <v>278</v>
+      </c>
+      <c r="B36" s="31"/>
+      <c r="C36" s="31"/>
+      <c r="D36" s="31"/>
+      <c r="E36" s="31"/>
       <c r="G36" t="s">
         <v>13</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="I36" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="7:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="31" t="s">
+        <v>280</v>
+      </c>
+      <c r="B37" s="31"/>
+      <c r="C37" s="31"/>
+      <c r="D37" s="31"/>
+      <c r="E37" s="31"/>
       <c r="G37" t="s">
         <v>14</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="I37" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="7:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="31" t="s">
+        <v>281</v>
+      </c>
+      <c r="B38" s="31"/>
+      <c r="C38" s="31"/>
+      <c r="D38" s="31"/>
+      <c r="E38" s="31"/>
       <c r="G38" t="s">
         <v>14</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="I38" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="7:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G39" t="s">
         <v>28</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="I39" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="7:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G40" t="s">
         <v>28</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="I40" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="7:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G41" t="s">
         <v>30</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="I41" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="7:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G42" t="s">
         <v>30</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="I42" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="7:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G43" t="s">
         <v>29</v>
       </c>
@@ -3635,7 +3749,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="44" spans="7:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G44" t="s">
         <v>29</v>
       </c>
@@ -3646,48 +3760,48 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="7:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G45" t="s">
         <v>33</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="J45" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="46" spans="7:10" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G46" t="s">
         <v>33</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="J46" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="47" spans="7:10" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G47" t="s">
         <v>15</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="J47" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="48" spans="7:10" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G48" t="s">
         <v>15</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="J48" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
     </row>
     <row r="49" spans="7:10" x14ac:dyDescent="0.25">
@@ -3695,10 +3809,10 @@
         <v>15</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="J49" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
     </row>
     <row r="50" spans="7:10" x14ac:dyDescent="0.25">
@@ -3706,10 +3820,10 @@
         <v>15</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="J50" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>

</xml_diff>